<commit_message>
added facings minimums to some blocking kpis
</commit_message>
<xml_diff>
--- a/Projects/RINIELSENUS/Data/Template_2018_v3.xlsx
+++ b/Projects/RINIELSENUS/Data/Template_2018_v3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Hierarchy" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,15 +34,19 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hierarchy!$A$1:$K$143</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Hierarchy!$A$1:$K$143</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Hierarchy!$A$1:$K$143</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Hierarchy!$A$1:$K$143</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">sales!$A$1:$E$71</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">sales!$A$1:$E$71</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">sales!$A$1:$E$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">sales!$A$1:$E$71</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">NBIL!$A$1:$F$1939</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">NBIL!$A$1:$F$1939</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">NBIL!$A$1:$F$1939</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">NBIL!$A$1:$F$1939</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Block!$A$1:$R$46</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Block!$A$1:$R$46</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Block!$A$1:$R$46</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Block!$A$1:$R$46</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">Adjacency!$A$1:$S$20</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">'Linear fair share'!$A$1:$I$22</definedName>
   </definedNames>
@@ -2328,22 +2332,22 @@
   <dimension ref="A1:K143"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A115" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="L49:L50 B3"/>
+      <selection pane="topLeft" activeCell="A147" activeCellId="0" sqref="A147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.4817813765182"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="99.085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="70.9109311740891"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="74.1255060728745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="99.9433198380567"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.4493927125506"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.2064777327935"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="51.7368421052632"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="52.165991902834"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6648,19 +6652,19 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L49:L50 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.3765182186235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.9109311740891"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
@@ -7149,17 +7153,17 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L49:L50 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.7004048582996"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.2348178137652"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7272,16 +7276,16 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L49:L50 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
@@ -7325,23 +7329,23 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L49:L50 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.9109311740891"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.4493927125506"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="110.975708502024"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="111.939271255061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.7813765182186"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
@@ -7433,17 +7437,17 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L49:L50 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.3846153846154"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.0566801619433"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.1740890688259"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
@@ -7512,14 +7516,14 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L49:L50 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7619,15 +7623,15 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L49:L50 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.7732793522267"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.3076923076923"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -7683,15 +7687,15 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L49:L50 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="10" width="6.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="8.89068825910931"/>
   </cols>
@@ -8803,25 +8807,25 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L49:L50 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.8056680161943"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.7773279352227"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.7732793522267"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="48.7408906882591"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.2429149797571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="30.3157894736842"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.3400809716599"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.8866396761134"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.2024291497976"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="49.165991902834"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="30.5303643724696"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.7813765182186"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9198,18 +9202,18 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L49:L50 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.7327935222672"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.3765182186235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
@@ -9282,19 +9286,19 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L49:L50 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.9473684210526"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.6963562753036"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
@@ -9726,17 +9730,17 @@
   <dimension ref="A1:F1939"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L49:L50 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.0283400809717"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.2429149797571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -40385,30 +40389,30 @@
   </sheetPr>
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L50" activeCellId="0" sqref="L49:L50"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.0566801619433"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.0971659919028"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="54.3076923076923"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="32.5627530364372"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="53.2388663967611"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="30.3157894736842"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="37.0647773279352"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.7004048582996"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.4210526315789"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="54.7368421052632"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="53.668016194332"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="30.5303643724696"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="37.3846153846154"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -40490,7 +40494,9 @@
       <c r="I2" s="29"/>
       <c r="J2" s="29"/>
       <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
+      <c r="L2" s="29" t="n">
+        <v>10</v>
+      </c>
       <c r="M2" s="29"/>
       <c r="N2" s="29" t="s">
         <v>42</v>
@@ -40876,7 +40882,9 @@
       <c r="I13" s="29"/>
       <c r="J13" s="29"/>
       <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
+      <c r="L13" s="29" t="n">
+        <v>10</v>
+      </c>
       <c r="M13" s="29"/>
       <c r="N13" s="29"/>
       <c r="O13" s="29" t="s">
@@ -42080,31 +42088,31 @@
   </sheetPr>
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L49:L50 A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="99.085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.8137651821862"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="99.9433198380567"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.8866396761134"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.1012145748988"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="48.7408906882591"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="30.3157894736842"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.3157894736842"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="49.165991902834"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="30.5303643724696"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -42981,22 +42989,22 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L49:L50 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.5263157894737"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="39.0971659919028"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="39.4210526315789"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.57085020242915"/>
   </cols>

</xml_diff>